<commit_message>
Update 25 Jan 24
</commit_message>
<xml_diff>
--- a/Capstone_Project/Data_Collection/job_postings_tech.xlsx
+++ b/Capstone_Project/Data_Collection/job_postings_tech.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27126"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/989c8b3702e2e0a7/Documents/GitHub/IBM_Data_Analytics/Capstone_Project/Data_Collection/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="2" documentId="11_6A69C497017A5406DD5410704B1510344D07F220" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{BDE2ACD6-1286-41C9-BD16-B6A1C859A071}"/>
+  <xr:revisionPtr revIDLastSave="3" documentId="11_6A69C497017A5406DD5410704B1510344D07F220" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{228A74F1-5442-46C4-9F33-6B8133FCB71D}"/>
   <bookViews>
-    <workbookView xWindow="7890" yWindow="2895" windowWidth="17280" windowHeight="12270" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView minimized="1" xWindow="780" yWindow="780" windowWidth="21600" windowHeight="11235" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet" sheetId="1" r:id="rId1"/>
@@ -22,9 +22,6 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
   <si>
-    <t>technology</t>
-  </si>
-  <si>
     <t>num_of_jobs</t>
   </si>
   <si>
@@ -62,6 +59,9 @@
   </si>
   <si>
     <t>MondaDB</t>
+  </si>
+  <si>
+    <t>Technology</t>
   </si>
 </sst>
 </file>
@@ -114,6 +114,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -403,7 +407,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G8" sqref="G8"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -413,15 +419,15 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B1" t="s">
         <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>1</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B2">
         <v>13498</v>
@@ -429,7 +435,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B3">
         <v>333</v>
@@ -437,7 +443,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B4">
         <v>13498</v>
@@ -445,7 +451,7 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B5">
         <v>2609</v>
@@ -453,7 +459,7 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B6">
         <v>355</v>
@@ -461,7 +467,7 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B7">
         <v>1173</v>
@@ -469,7 +475,7 @@
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B8">
         <v>33</v>
@@ -477,7 +483,7 @@
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B9">
         <v>784</v>
@@ -485,7 +491,7 @@
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B10">
         <v>250</v>
@@ -493,7 +499,7 @@
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B11">
         <v>0</v>
@@ -501,7 +507,7 @@
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B12">
         <v>10</v>
@@ -509,7 +515,7 @@
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B13">
         <v>0</v>

</xml_diff>